<commit_message>
Allow for selection of starting model ID based on definition in Instance Tab.
Allow for selection of starting model ID based on definition in "Instance" Tab. The starting model ID is defined in the "Instance" Tab. Details on the starting_comparative_model can then be given in the "Starting_comparative_model" tab.
</commit_message>
<xml_diff>
--- a/example/excel_example.xlsx
+++ b/example/excel_example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\git_directory\excel2mmcif\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\tmp_excel2mmcif_working_directory\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3378,7 +3378,7 @@
   <dimension ref="A2:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B10"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8480,9 +8480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8940,7 +8938,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B5" sqref="B5:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9065,7 +9063,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J1048576">
       <formula1>"Length of the shorter sequence, Number of aligned positions (including gaps), Number of aligned residue pairs (not including gaps), Arithmetic mean sequence length, Other"</formula1>
     </dataValidation>
@@ -9074,6 +9072,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L5:L1048576">
       <formula1>external_file_id</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:B1048576">
+      <formula1>starting_model_id</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix typo in excel templates.
Fix typo in excel templates.
</commit_message>
<xml_diff>
--- a/example/excel_example.xlsx
+++ b/example/excel_example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\tmp_excel2mmcif_working_directory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\git_directory\excel2mmcif\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2303,9 +2303,6 @@
     <t>Is the data deposited in a database? (yes/no)</t>
   </si>
   <si>
-    <t>An identifier used to connect to the external files given in the 'External_files' tab. Please give unique identifier here.</t>
-  </si>
-  <si>
     <t>What does the reference refer to? Please select.</t>
   </si>
   <si>
@@ -2399,9 +2396,6 @@
     <t>The dataset list ID (Tab 'Dataset')</t>
   </si>
   <si>
-    <t>How was the starting model obtained? (In case of 'comparative model', referes to Tab 'Starting_comparative_model')</t>
-  </si>
-  <si>
     <t>An ID for the step in the modeling protocol</t>
   </si>
   <si>
@@ -2859,6 +2853,12 @@
   </si>
   <si>
     <t>Each row has a unique ID in the first column. This has to be filled.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An identifier used to connect to the external files given in the 'External_files' tab. </t>
+  </si>
+  <si>
+    <t>How was the starting model obtained? (In case of 'comparative model', refers to Tab 'Starting_comparative_model')</t>
   </si>
 </sst>
 </file>
@@ -3378,14 +3378,14 @@
   <dimension ref="A2:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3393,7 +3393,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3401,7 +3401,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3409,7 +3409,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3417,7 +3417,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3425,7 +3425,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -3433,7 +3433,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -3441,7 +3441,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -3449,7 +3449,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
     </row>
   </sheetData>
@@ -3469,7 +3469,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="22" customFormat="1" ht="157.5" x14ac:dyDescent="0.25">
@@ -3477,37 +3477,37 @@
         <v>739</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>786</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>858</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>787</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>859</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>860</v>
+      </c>
+      <c r="G2" s="22" t="s">
         <v>788</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>860</v>
-      </c>
-      <c r="D2" s="22" t="s">
+      <c r="H2" s="22" t="s">
         <v>789</v>
       </c>
-      <c r="E2" s="22" t="s">
-        <v>861</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>862</v>
-      </c>
-      <c r="G2" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>790</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>791</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>792</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="L2" s="22" t="s">
         <v>793</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>794</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>795</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
@@ -3612,7 +3612,7 @@
         <v>162</v>
       </c>
       <c r="I5" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="L5">
         <v>2</v>
@@ -3663,7 +3663,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="22" customFormat="1" ht="63" x14ac:dyDescent="0.25">
@@ -3671,28 +3671,28 @@
         <v>739</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>794</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>795</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>862</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>796</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>797</v>
       </c>
-      <c r="D2" s="22" t="s">
-        <v>864</v>
-      </c>
-      <c r="E2" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>798</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="H2" s="22" t="s">
+        <v>863</v>
+      </c>
+      <c r="I2" s="22" t="s">
         <v>799</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>800</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>865</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>801</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
@@ -3836,7 +3836,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="22" customFormat="1" ht="173.25" x14ac:dyDescent="0.25">
@@ -3844,34 +3844,34 @@
         <v>739</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>800</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>801</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>802</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="E2" s="22" t="s">
+        <v>865</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>866</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>867</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>868</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>869</v>
+      </c>
+      <c r="J2" s="22" t="s">
         <v>803</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>804</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>867</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>868</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>869</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>870</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>871</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>805</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>806</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="63" hidden="1" x14ac:dyDescent="0.25">
@@ -4346,7 +4346,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="22" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
@@ -4354,31 +4354,31 @@
         <v>739</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>805</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>871</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>872</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>806</v>
+      </c>
+      <c r="F2" s="22" t="s">
         <v>807</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>873</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>874</v>
-      </c>
-      <c r="E2" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>808</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="H2" s="22" t="s">
         <v>809</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>810</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>811</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>812</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>813</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="1" customFormat="1" ht="110.25" hidden="1" x14ac:dyDescent="0.25">
@@ -4450,7 +4450,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -4476,7 +4476,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -4549,7 +4549,7 @@
   <sheetData>
     <row r="1" spans="1:114" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="23" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="B1" s="26"/>
       <c r="E1" s="26"/>
@@ -4572,7 +4572,7 @@
     </row>
     <row r="2" spans="1:114" s="9" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="B2" s="19" t="s">
         <v>183</v>
@@ -4725,7 +4725,7 @@
       </c>
       <c r="C3" s="24"/>
       <c r="D3" s="24" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="E3" s="25" t="s">
         <v>201</v>
@@ -4741,10 +4741,10 @@
         <v>203</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="K3" s="24" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="L3" s="25" t="s">
         <v>204</v>
@@ -5294,37 +5294,37 @@
         <v>370</v>
       </c>
       <c r="CD4" s="16" t="s">
+        <v>877</v>
+      </c>
+      <c r="CE4" s="15" t="s">
+        <v>878</v>
+      </c>
+      <c r="CF4" s="15" t="s">
         <v>879</v>
       </c>
-      <c r="CE4" s="15" t="s">
+      <c r="CG4" s="15" t="s">
         <v>880</v>
       </c>
-      <c r="CF4" s="15" t="s">
+      <c r="CH4" s="15" t="s">
         <v>881</v>
       </c>
-      <c r="CG4" s="15" t="s">
+      <c r="CI4" s="15" t="s">
         <v>882</v>
       </c>
-      <c r="CH4" s="15" t="s">
+      <c r="CJ4" s="15" t="s">
         <v>883</v>
       </c>
-      <c r="CI4" s="15" t="s">
+      <c r="CK4" s="15" t="s">
         <v>884</v>
       </c>
-      <c r="CJ4" s="15" t="s">
+      <c r="CL4" s="15" t="s">
         <v>885</v>
       </c>
-      <c r="CK4" s="15" t="s">
+      <c r="CM4" s="15" t="s">
         <v>886</v>
       </c>
-      <c r="CL4" s="15" t="s">
+      <c r="CN4" s="9" t="s">
         <v>887</v>
-      </c>
-      <c r="CM4" s="15" t="s">
-        <v>888</v>
-      </c>
-      <c r="CN4" s="9" t="s">
-        <v>889</v>
       </c>
       <c r="CP4" s="16" t="s">
         <v>371</v>
@@ -5399,7 +5399,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="E5" s="4">
         <v>2</v>
@@ -5408,15 +5408,15 @@
         <v>178</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
       <c r="J5" s="7" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>383</v>
@@ -5464,7 +5464,7 @@
         <v>394</v>
       </c>
       <c r="AC5" s="7" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="AD5" s="5"/>
       <c r="AE5" s="5" t="s">
@@ -5507,7 +5507,7 @@
         <v>176</v>
       </c>
       <c r="AV5" s="5" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="AW5" s="5">
         <v>1</v>
@@ -5528,13 +5528,13 @@
         <v>176</v>
       </c>
       <c r="BC5" s="5" t="s">
+        <v>912</v>
+      </c>
+      <c r="BD5" s="4" t="s">
+        <v>913</v>
+      </c>
+      <c r="BE5" s="5" t="s">
         <v>914</v>
-      </c>
-      <c r="BD5" s="4" t="s">
-        <v>915</v>
-      </c>
-      <c r="BE5" s="5" t="s">
-        <v>916</v>
       </c>
       <c r="BF5" s="4" t="s">
         <v>399</v>
@@ -5675,7 +5675,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="E6" s="4">
         <v>2</v>
@@ -5684,15 +5684,15 @@
         <v>178</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="7" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>383</v>
@@ -5740,7 +5740,7 @@
         <v>394</v>
       </c>
       <c r="AC6" s="7" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="AD6" s="5"/>
       <c r="AE6" s="5" t="s">
@@ -5783,7 +5783,7 @@
         <v>176</v>
       </c>
       <c r="AV6" s="5" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="AW6" s="5">
         <v>1</v>
@@ -5804,13 +5804,13 @@
         <v>176</v>
       </c>
       <c r="BC6" s="5" t="s">
+        <v>912</v>
+      </c>
+      <c r="BD6" s="4" t="s">
+        <v>913</v>
+      </c>
+      <c r="BE6" s="5" t="s">
         <v>914</v>
-      </c>
-      <c r="BD6" s="4" t="s">
-        <v>915</v>
-      </c>
-      <c r="BE6" s="5" t="s">
-        <v>916</v>
       </c>
       <c r="BF6" s="4" t="s">
         <v>399</v>
@@ -6195,7 +6195,7 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="22" customFormat="1" ht="173.25" x14ac:dyDescent="0.25">
@@ -6203,13 +6203,13 @@
         <v>739</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>813</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>814</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>815</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>816</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>817</v>
       </c>
     </row>
     <row r="3" spans="1:22" hidden="1" x14ac:dyDescent="0.25">
@@ -6291,7 +6291,7 @@
         <v>532</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>531</v>
@@ -6520,7 +6520,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="22" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
@@ -6528,13 +6528,13 @@
         <v>739</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
     </row>
     <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
@@ -6870,7 +6870,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="22" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
@@ -6878,19 +6878,19 @@
         <v>739</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>816</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>817</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>876</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>818</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>819</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>878</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>820</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>821</v>
       </c>
     </row>
     <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
@@ -7449,7 +7449,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
     </row>
     <row r="2" spans="1:10" s="22" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
@@ -7457,7 +7457,7 @@
         <v>739</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="C2" s="22" t="s">
         <v>735</v>
@@ -7553,10 +7553,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
     </row>
   </sheetData>
@@ -7592,7 +7592,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="22" customFormat="1" ht="299.25" x14ac:dyDescent="0.25">
@@ -7600,40 +7600,40 @@
         <v>739</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>750</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>751</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="D2" s="22" t="s">
         <v>752</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="E2" s="22" t="s">
         <v>753</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="22" t="s">
+        <v>837</v>
+      </c>
+      <c r="G2" s="22" t="s">
         <v>754</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="H2" s="22" t="s">
+        <v>755</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>756</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>757</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>758</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>838</v>
+      </c>
+      <c r="M2" s="22" t="s">
         <v>839</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>755</v>
-      </c>
-      <c r="H2" s="22" t="s">
-        <v>756</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>757</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>758</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>759</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>840</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>841</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="63" hidden="1" x14ac:dyDescent="0.25">
@@ -7879,7 +7879,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:I10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7893,10 +7895,10 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" s="22" customFormat="1" ht="189.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="22" customFormat="1" ht="174" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="22" t="s">
         <v>739</v>
       </c>
@@ -7904,43 +7906,43 @@
         <v>740</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="D2" s="22" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="E2" s="22" t="s">
         <v>741</v>
       </c>
       <c r="F2" s="22" t="s">
+        <v>828</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>829</v>
+      </c>
+      <c r="H2" s="22" t="s">
         <v>830</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="I2" s="22" t="s">
+        <v>926</v>
+      </c>
+      <c r="J2" s="22" t="s">
         <v>831</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>832</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="L2" s="22" t="s">
+        <v>833</v>
+      </c>
+      <c r="M2" s="22" t="s">
         <v>742</v>
       </c>
-      <c r="J2" s="22" t="s">
-        <v>833</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>834</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>835</v>
-      </c>
-      <c r="M2" s="22" t="s">
+      <c r="N2" s="22" t="s">
         <v>743</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="O2" s="22" t="s">
         <v>744</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="48" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -8078,7 +8080,7 @@
         <v>504</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -8119,7 +8121,7 @@
         <v>505</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
     </row>
   </sheetData>
@@ -8182,7 +8184,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="22" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
@@ -8190,22 +8192,22 @@
         <v>739</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>745</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>840</v>
+      </c>
+      <c r="D2" s="22" t="s">
         <v>746</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>842</v>
-      </c>
-      <c r="D2" s="22" t="s">
+      <c r="E2" s="22" t="s">
         <v>747</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="F2" s="22" t="s">
         <v>748</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>749</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>750</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
@@ -8262,7 +8264,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="D5" t="s">
         <v>86</v>
@@ -8271,7 +8273,7 @@
         <v>106</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -8282,7 +8284,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="D6" t="s">
         <v>86</v>
@@ -8291,7 +8293,7 @@
         <v>106</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="19.899999999999999" customHeight="1" x14ac:dyDescent="0.25">
@@ -8302,7 +8304,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="D7" t="s">
         <v>86</v>
@@ -8311,7 +8313,7 @@
         <v>106</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -8376,7 +8378,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="22" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
@@ -8480,7 +8482,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8492,7 +8496,7 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
     </row>
     <row r="2" spans="1:28" s="22" customFormat="1" ht="110.25" x14ac:dyDescent="0.25">
@@ -8500,58 +8504,58 @@
         <v>739</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>841</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>842</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>761</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>843</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="F2" s="22" t="s">
+        <v>762</v>
+      </c>
+      <c r="G2" s="22" t="s">
         <v>844</v>
       </c>
-      <c r="D2" s="22" t="s">
-        <v>762</v>
-      </c>
-      <c r="E2" s="22" t="s">
+      <c r="H2" s="22" t="s">
+        <v>764</v>
+      </c>
+      <c r="I2" s="22" t="s">
         <v>845</v>
       </c>
-      <c r="F2" s="22" t="s">
-        <v>763</v>
-      </c>
-      <c r="G2" s="22" t="s">
+      <c r="J2" s="22" t="s">
+        <v>765</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>766</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>767</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>768</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>769</v>
+      </c>
+      <c r="O2" s="22" t="s">
         <v>846</v>
       </c>
-      <c r="H2" s="22" t="s">
-        <v>765</v>
-      </c>
-      <c r="I2" s="22" t="s">
-        <v>847</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>766</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>767</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>768</v>
-      </c>
-      <c r="M2" s="22" t="s">
-        <v>769</v>
-      </c>
-      <c r="N2" s="22" t="s">
+      <c r="P2" s="22" t="s">
+        <v>927</v>
+      </c>
+      <c r="Q2" s="22" t="s">
         <v>770</v>
       </c>
-      <c r="O2" s="22" t="s">
-        <v>848</v>
-      </c>
-      <c r="P2" s="22" t="s">
-        <v>774</v>
-      </c>
-      <c r="Q2" s="22" t="s">
+      <c r="R2" s="22" t="s">
         <v>771</v>
       </c>
-      <c r="R2" s="22" t="s">
+      <c r="S2" s="22" t="s">
         <v>772</v>
-      </c>
-      <c r="S2" s="22" t="s">
-        <v>773</v>
       </c>
     </row>
     <row r="3" spans="1:28" ht="63" hidden="1" x14ac:dyDescent="0.25">
@@ -8692,7 +8696,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -8704,10 +8708,10 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -8748,7 +8752,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -8760,10 +8764,10 @@
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -8804,7 +8808,7 @@
         <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -8816,10 +8820,10 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -8860,7 +8864,7 @@
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -8872,10 +8876,10 @@
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -8953,37 +8957,37 @@
         <v>739</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>759</v>
+      </c>
+      <c r="C2" s="22" t="s">
         <v>760</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>761</v>
-      </c>
       <c r="D2" s="22" t="s">
+        <v>847</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>848</v>
+      </c>
+      <c r="F2" s="22" t="s">
         <v>849</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="G2" s="22" t="s">
         <v>850</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="H2" s="22" t="s">
         <v>851</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>852</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>853</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>854</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="L2" s="22" t="s">
         <v>855</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>856</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>857</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="78.75" hidden="1" x14ac:dyDescent="0.25">
@@ -9097,7 +9101,7 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="22" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
@@ -9105,46 +9109,46 @@
         <v>739</v>
       </c>
       <c r="B2" s="22" t="s">
+        <v>774</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>773</v>
+      </c>
+      <c r="D2" s="22" t="s">
+        <v>856</v>
+      </c>
+      <c r="E2" s="22" t="s">
+        <v>857</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>775</v>
+      </c>
+      <c r="G2" s="22" t="s">
         <v>776</v>
       </c>
-      <c r="C2" s="22" t="s">
-        <v>775</v>
-      </c>
-      <c r="D2" s="22" t="s">
-        <v>858</v>
-      </c>
-      <c r="E2" s="22" t="s">
-        <v>859</v>
-      </c>
-      <c r="F2" s="22" t="s">
+      <c r="H2" s="22" t="s">
         <v>777</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="I2" s="22" t="s">
         <v>778</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="J2" s="22" t="s">
         <v>779</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="K2" s="22" t="s">
         <v>780</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="L2" s="22" t="s">
         <v>781</v>
       </c>
-      <c r="K2" s="22" t="s">
+      <c r="M2" s="22" t="s">
         <v>782</v>
       </c>
-      <c r="L2" s="22" t="s">
+      <c r="N2" s="22" t="s">
         <v>783</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="O2" s="22" t="s">
         <v>784</v>
-      </c>
-      <c r="N2" s="22" t="s">
-        <v>785</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>786</v>
       </c>
     </row>
     <row r="3" spans="1:15" s="1" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add processing of entry title
Add processing of entry title (Tab General in excel sheet)
</commit_message>
<xml_diff>
--- a/example/excel_example.xlsx
+++ b/example/excel_example.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HankeC\work\for_PDB\excel2mmcif\20191031_excel2mmcif_addition_of_lifetime_based_analysis\20191106_preparation_of_T4L_files\raw_files_for_excel2mmcif\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\excel2mmcif_working_directory\tmp_directory_for_comparison\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,30 +13,31 @@
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="19" r:id="rId1"/>
-    <sheet name="Citation" sheetId="14" r:id="rId2"/>
-    <sheet name="Entity" sheetId="1" r:id="rId3"/>
-    <sheet name="Dataset" sheetId="4" r:id="rId4"/>
-    <sheet name="External_files" sheetId="5" r:id="rId5"/>
-    <sheet name="Software" sheetId="13" r:id="rId6"/>
-    <sheet name="Instance" sheetId="3" r:id="rId7"/>
-    <sheet name="Starting_comparative_model" sheetId="16" r:id="rId8"/>
-    <sheet name="Modeling_protocol" sheetId="6" r:id="rId9"/>
-    <sheet name="Modeling_post_process" sheetId="15" r:id="rId10"/>
-    <sheet name="Multi-state modeling" sheetId="7" r:id="rId11"/>
-    <sheet name="Models" sheetId="2" r:id="rId12"/>
-    <sheet name="Ensemble Info" sheetId="17" r:id="rId13"/>
-    <sheet name="Reference_measurements" sheetId="20" r:id="rId14"/>
-    <sheet name="FLR" sheetId="8" r:id="rId15"/>
-    <sheet name="FLR_FPS_MPP_group" sheetId="18" r:id="rId16"/>
-    <sheet name="FLR_FPS_global_parameters" sheetId="12" r:id="rId17"/>
-    <sheet name="FLR_FRET_Model_distances" sheetId="10" r:id="rId18"/>
-    <sheet name="FLR_FRET_Model_quality" sheetId="11" r:id="rId19"/>
-    <sheet name="for_internal_use_only" sheetId="9" state="hidden" r:id="rId20"/>
+    <sheet name="General" sheetId="21" r:id="rId2"/>
+    <sheet name="Citation" sheetId="14" r:id="rId3"/>
+    <sheet name="Entity" sheetId="1" r:id="rId4"/>
+    <sheet name="Dataset" sheetId="4" r:id="rId5"/>
+    <sheet name="External_files" sheetId="5" r:id="rId6"/>
+    <sheet name="Software" sheetId="13" r:id="rId7"/>
+    <sheet name="Instance" sheetId="3" r:id="rId8"/>
+    <sheet name="Starting_comparative_model" sheetId="16" r:id="rId9"/>
+    <sheet name="Modeling_protocol" sheetId="6" r:id="rId10"/>
+    <sheet name="Modeling_post_process" sheetId="15" r:id="rId11"/>
+    <sheet name="Multi-state modeling" sheetId="7" r:id="rId12"/>
+    <sheet name="Models" sheetId="2" r:id="rId13"/>
+    <sheet name="Ensemble Info" sheetId="17" r:id="rId14"/>
+    <sheet name="Reference_measurements" sheetId="20" r:id="rId15"/>
+    <sheet name="FLR" sheetId="8" r:id="rId16"/>
+    <sheet name="FLR_FPS_MPP_group" sheetId="18" r:id="rId17"/>
+    <sheet name="FLR_FPS_global_parameters" sheetId="12" r:id="rId18"/>
+    <sheet name="FLR_FRET_Model_distances" sheetId="10" r:id="rId19"/>
+    <sheet name="FLR_FRET_Model_quality" sheetId="11" r:id="rId20"/>
+    <sheet name="for_internal_use_only" sheetId="9" state="hidden" r:id="rId21"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId21"/>
     <externalReference r:id="rId22"/>
     <externalReference r:id="rId23"/>
+    <externalReference r:id="rId24"/>
   </externalReferences>
   <definedNames>
     <definedName name="citation_id">Citation!$A$5:$A$1048576</definedName>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1341" uniqueCount="1044">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="1049">
   <si>
     <t>Model number</t>
   </si>
@@ -3209,6 +3210,21 @@
   </si>
   <si>
     <t>"^2"</t>
+  </si>
+  <si>
+    <t>Description the entry</t>
+  </si>
+  <si>
+    <t>Title of the entry</t>
+  </si>
+  <si>
+    <t>IHM_Struct_id</t>
+  </si>
+  <si>
+    <t>IHM_Struct_title</t>
+  </si>
+  <si>
+    <t>Title of the entry is given here.</t>
   </si>
 </sst>
 </file>
@@ -4148,7 +4164,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4233,6 +4249,275 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="9" width="17.25" customWidth="1"/>
+    <col min="10" max="10" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="20" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>654</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>689</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>688</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>771</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>772</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>690</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>691</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>692</v>
+      </c>
+      <c r="I2" s="20" t="s">
+        <v>693</v>
+      </c>
+      <c r="J2" s="20" t="s">
+        <v>694</v>
+      </c>
+      <c r="K2" s="20" t="s">
+        <v>695</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>696</v>
+      </c>
+      <c r="M2" s="20" t="s">
+        <v>697</v>
+      </c>
+      <c r="N2" s="20" t="s">
+        <v>698</v>
+      </c>
+      <c r="O2" s="20" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" s="11" customFormat="1" ht="63" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
+        <v>399</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>401</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>400</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>402</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>403</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>404</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>405</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>406</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>407</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>408</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>409</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>410</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>411</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="84">
+        <v>1</v>
+      </c>
+      <c r="B5" s="84">
+        <v>1</v>
+      </c>
+      <c r="C5" s="84">
+        <v>1</v>
+      </c>
+      <c r="D5" s="84">
+        <v>1</v>
+      </c>
+      <c r="E5" s="84">
+        <v>1</v>
+      </c>
+      <c r="F5" s="84" t="s">
+        <v>991</v>
+      </c>
+      <c r="G5" s="84" t="s">
+        <v>992</v>
+      </c>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84">
+        <v>0</v>
+      </c>
+      <c r="J5" s="84">
+        <v>1000</v>
+      </c>
+      <c r="K5" s="84" t="s">
+        <v>993</v>
+      </c>
+      <c r="L5" s="84" t="s">
+        <v>994</v>
+      </c>
+      <c r="M5" s="84" t="s">
+        <v>993</v>
+      </c>
+      <c r="N5" s="84" t="s">
+        <v>994</v>
+      </c>
+      <c r="O5" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="84">
+        <v>2</v>
+      </c>
+      <c r="B6" s="84">
+        <v>1</v>
+      </c>
+      <c r="C6" s="84">
+        <v>2</v>
+      </c>
+      <c r="D6" s="84">
+        <v>1</v>
+      </c>
+      <c r="E6" s="84">
+        <v>1</v>
+      </c>
+      <c r="F6" s="84" t="s">
+        <v>991</v>
+      </c>
+      <c r="G6" s="84" t="s">
+        <v>995</v>
+      </c>
+      <c r="H6" s="84"/>
+      <c r="I6" s="84">
+        <v>1000</v>
+      </c>
+      <c r="J6" s="84">
+        <v>1000</v>
+      </c>
+      <c r="K6" s="84" t="s">
+        <v>993</v>
+      </c>
+      <c r="L6" s="84" t="s">
+        <v>994</v>
+      </c>
+      <c r="M6" s="84" t="s">
+        <v>993</v>
+      </c>
+      <c r="N6" s="84" t="s">
+        <v>994</v>
+      </c>
+      <c r="O6" s="84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O8" s="2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O1048576">
+      <formula1>Software_id</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E1048576">
+      <formula1>Dataset_group_id</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D1048576">
+      <formula1>structure_assembly_id</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
@@ -4420,7 +4705,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
@@ -4613,7 +4898,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K15"/>
   <sheetViews>
@@ -5114,7 +5399,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
@@ -5312,7 +5597,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR82"/>
   <sheetViews>
@@ -8167,7 +8452,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DR204"/>
   <sheetViews>
@@ -32139,7 +32424,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
@@ -32229,7 +32514,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V7"/>
   <sheetViews>
@@ -32554,7 +32839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
@@ -32904,7 +33189,58 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B1" s="113"/>
+    </row>
+    <row r="2" spans="1:2" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="76" t="s">
+        <v>654</v>
+      </c>
+      <c r="B2" s="76" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="113"/>
+      <c r="B3" s="113" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="71" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B4" s="71" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
@@ -33157,7 +33493,330 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" t="s">
+        <v>139</v>
+      </c>
+      <c r="G1" t="s">
+        <v>389</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" t="s">
+        <v>142</v>
+      </c>
+      <c r="G2" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G3" t="s">
+        <v>90</v>
+      </c>
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" t="s">
+        <v>91</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>92</v>
+      </c>
+      <c r="K5" t="s">
+        <v>41</v>
+      </c>
+      <c r="L5" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>93</v>
+      </c>
+      <c r="K6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N6" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>94</v>
+      </c>
+      <c r="K7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" t="s">
+        <v>61</v>
+      </c>
+      <c r="N7" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>95</v>
+      </c>
+      <c r="K8" t="s">
+        <v>44</v>
+      </c>
+      <c r="L8" t="s">
+        <v>62</v>
+      </c>
+      <c r="N8" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>96</v>
+      </c>
+      <c r="K9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N9" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10" t="s">
+        <v>46</v>
+      </c>
+      <c r="L10" t="s">
+        <v>64</v>
+      </c>
+      <c r="N10" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>98</v>
+      </c>
+      <c r="K11" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11" t="s">
+        <v>65</v>
+      </c>
+      <c r="N11" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>85</v>
+      </c>
+      <c r="K12" t="s">
+        <v>38</v>
+      </c>
+      <c r="L12" t="s">
+        <v>66</v>
+      </c>
+      <c r="N12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K13" t="s">
+        <v>37</v>
+      </c>
+      <c r="L13" t="s">
+        <v>56</v>
+      </c>
+      <c r="N13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
+        <v>48</v>
+      </c>
+      <c r="L14" t="s">
+        <v>85</v>
+      </c>
+      <c r="N14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K15" t="s">
+        <v>49</v>
+      </c>
+      <c r="N15" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="K16" t="s">
+        <v>50</v>
+      </c>
+      <c r="N16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K17" t="s">
+        <v>51</v>
+      </c>
+      <c r="N17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K18" t="s">
+        <v>52</v>
+      </c>
+      <c r="N18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K19" t="s">
+        <v>53</v>
+      </c>
+      <c r="N19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K20" t="s">
+        <v>54</v>
+      </c>
+      <c r="N20" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K21" t="s">
+        <v>55</v>
+      </c>
+      <c r="N21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="K22" t="s">
+        <v>56</v>
+      </c>
+      <c r="N22" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J5"/>
   <sheetViews>
@@ -33287,330 +33946,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" t="s">
-        <v>389</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N1" t="s">
-        <v>395</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E2" t="s">
-        <v>142</v>
-      </c>
-      <c r="G2" t="s">
-        <v>89</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C3" t="s">
-        <v>144</v>
-      </c>
-      <c r="E3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G3" t="s">
-        <v>90</v>
-      </c>
-      <c r="K3" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>146</v>
-      </c>
-      <c r="E4" t="s">
-        <v>90</v>
-      </c>
-      <c r="G4" t="s">
-        <v>91</v>
-      </c>
-      <c r="K4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" t="s">
-        <v>58</v>
-      </c>
-      <c r="N4" t="s">
-        <v>68</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G5" t="s">
-        <v>92</v>
-      </c>
-      <c r="K5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L5" t="s">
-        <v>59</v>
-      </c>
-      <c r="N5" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G6" t="s">
-        <v>93</v>
-      </c>
-      <c r="K6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L6" t="s">
-        <v>60</v>
-      </c>
-      <c r="N6" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>535</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G7" t="s">
-        <v>94</v>
-      </c>
-      <c r="K7" t="s">
-        <v>43</v>
-      </c>
-      <c r="L7" t="s">
-        <v>61</v>
-      </c>
-      <c r="N7" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G8" t="s">
-        <v>95</v>
-      </c>
-      <c r="K8" t="s">
-        <v>44</v>
-      </c>
-      <c r="L8" t="s">
-        <v>62</v>
-      </c>
-      <c r="N8" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="G9" t="s">
-        <v>96</v>
-      </c>
-      <c r="K9" t="s">
-        <v>45</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="N9" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G10" t="s">
-        <v>97</v>
-      </c>
-      <c r="K10" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" t="s">
-        <v>64</v>
-      </c>
-      <c r="N10" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G11" t="s">
-        <v>98</v>
-      </c>
-      <c r="K11" t="s">
-        <v>47</v>
-      </c>
-      <c r="L11" t="s">
-        <v>65</v>
-      </c>
-      <c r="N11" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="G12" t="s">
-        <v>85</v>
-      </c>
-      <c r="K12" t="s">
-        <v>38</v>
-      </c>
-      <c r="L12" t="s">
-        <v>66</v>
-      </c>
-      <c r="N12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K13" t="s">
-        <v>37</v>
-      </c>
-      <c r="L13" t="s">
-        <v>56</v>
-      </c>
-      <c r="N13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K14" t="s">
-        <v>48</v>
-      </c>
-      <c r="L14" t="s">
-        <v>85</v>
-      </c>
-      <c r="N14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K15" t="s">
-        <v>49</v>
-      </c>
-      <c r="N15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="K16" t="s">
-        <v>50</v>
-      </c>
-      <c r="N16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K17" t="s">
-        <v>51</v>
-      </c>
-      <c r="N17" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K18" t="s">
-        <v>52</v>
-      </c>
-      <c r="N18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="19" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K19" t="s">
-        <v>53</v>
-      </c>
-      <c r="N19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K20" t="s">
-        <v>54</v>
-      </c>
-      <c r="N20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K21" t="s">
-        <v>55</v>
-      </c>
-      <c r="N21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="11:14" x14ac:dyDescent="0.25">
-      <c r="K22" t="s">
-        <v>56</v>
-      </c>
-      <c r="N22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P38"/>
   <sheetViews>
@@ -34048,7 +34384,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U8"/>
   <sheetViews>
@@ -34388,7 +34724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H202"/>
   <sheetViews>
@@ -35142,7 +35478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G37"/>
   <sheetViews>
@@ -35354,7 +35690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB13"/>
   <sheetViews>
@@ -35841,7 +36177,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
@@ -36051,273 +36387,4 @@
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="9" max="9" width="17.25" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="20" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
-        <v>654</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>689</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>688</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>771</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>772</v>
-      </c>
-      <c r="F2" s="20" t="s">
-        <v>690</v>
-      </c>
-      <c r="G2" s="20" t="s">
-        <v>691</v>
-      </c>
-      <c r="H2" s="20" t="s">
-        <v>692</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>693</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>694</v>
-      </c>
-      <c r="K2" s="20" t="s">
-        <v>695</v>
-      </c>
-      <c r="L2" s="20" t="s">
-        <v>696</v>
-      </c>
-      <c r="M2" s="20" t="s">
-        <v>697</v>
-      </c>
-      <c r="N2" s="20" t="s">
-        <v>698</v>
-      </c>
-      <c r="O2" s="20" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="31.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="11" customFormat="1" ht="63" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>399</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>401</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>400</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>412</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>402</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>403</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>404</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>405</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>406</v>
-      </c>
-      <c r="J4" s="11" t="s">
-        <v>407</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>408</v>
-      </c>
-      <c r="L4" s="11" t="s">
-        <v>409</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>410</v>
-      </c>
-      <c r="N4" s="11" t="s">
-        <v>411</v>
-      </c>
-      <c r="O4" s="11" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="84">
-        <v>1</v>
-      </c>
-      <c r="B5" s="84">
-        <v>1</v>
-      </c>
-      <c r="C5" s="84">
-        <v>1</v>
-      </c>
-      <c r="D5" s="84">
-        <v>1</v>
-      </c>
-      <c r="E5" s="84">
-        <v>1</v>
-      </c>
-      <c r="F5" s="84" t="s">
-        <v>991</v>
-      </c>
-      <c r="G5" s="84" t="s">
-        <v>992</v>
-      </c>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84">
-        <v>0</v>
-      </c>
-      <c r="J5" s="84">
-        <v>1000</v>
-      </c>
-      <c r="K5" s="84" t="s">
-        <v>993</v>
-      </c>
-      <c r="L5" s="84" t="s">
-        <v>994</v>
-      </c>
-      <c r="M5" s="84" t="s">
-        <v>993</v>
-      </c>
-      <c r="N5" s="84" t="s">
-        <v>994</v>
-      </c>
-      <c r="O5" s="84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="84">
-        <v>2</v>
-      </c>
-      <c r="B6" s="84">
-        <v>1</v>
-      </c>
-      <c r="C6" s="84">
-        <v>2</v>
-      </c>
-      <c r="D6" s="84">
-        <v>1</v>
-      </c>
-      <c r="E6" s="84">
-        <v>1</v>
-      </c>
-      <c r="F6" s="84" t="s">
-        <v>991</v>
-      </c>
-      <c r="G6" s="84" t="s">
-        <v>995</v>
-      </c>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84">
-        <v>1000</v>
-      </c>
-      <c r="J6" s="84">
-        <v>1000</v>
-      </c>
-      <c r="K6" s="84" t="s">
-        <v>993</v>
-      </c>
-      <c r="L6" s="84" t="s">
-        <v>994</v>
-      </c>
-      <c r="M6" s="84" t="s">
-        <v>993</v>
-      </c>
-      <c r="N6" s="84" t="s">
-        <v>994</v>
-      </c>
-      <c r="O6" s="84">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="O8" s="2"/>
-    </row>
-  </sheetData>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O1048576">
-      <formula1>Software_id</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E1048576">
-      <formula1>Dataset_group_id</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D1048576">
-      <formula1>structure_assembly_id</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update to excel sheets
Update to excel sheets
</commit_message>
<xml_diff>
--- a/example/excel_example.xlsx
+++ b/example/excel_example.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\excel2mmcif_working_directory\excel2mmcif_20200227\test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\git_directory\excel2mmcif\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="730" firstSheet="12" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="730"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="19" r:id="rId1"/>
@@ -4246,8 +4246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5685,7 +5685,7 @@
   <dimension ref="A1:BT82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5706,7 +5706,9 @@
     <col min="32" max="32" width="11" style="18" customWidth="1"/>
     <col min="33" max="35" width="11" customWidth="1"/>
     <col min="36" max="36" width="11" style="74" customWidth="1"/>
-    <col min="37" max="43" width="11" style="111" customWidth="1"/>
+    <col min="37" max="39" width="11" style="111" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="11" style="111" customWidth="1"/>
+    <col min="41" max="43" width="11" style="111" hidden="1" customWidth="1"/>
     <col min="44" max="44" width="11" style="18" customWidth="1"/>
     <col min="45" max="57" width="11" customWidth="1"/>
     <col min="58" max="58" width="11" style="74" customWidth="1"/>
@@ -8760,9 +8762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DT204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BZ4" workbookViewId="0">
-      <selection activeCell="CN8" sqref="CN8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Fix internal referencing in excel sheet
Fix internal referencing in excel sheets
</commit_message>
<xml_diff>
--- a/example/excel_example.xlsx
+++ b/example/excel_example.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\HankeC\work\for_PDB\excel2mmcif\20230216_excel2mmcif_devel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\excel2mmcif\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D78DB937-22F4-4218-8796-96B6BBB8AE90}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5189C1-F95B-4EDA-928A-AE314F4C6A39}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9420" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4635,7 +4635,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -36589,7 +36589,7 @@
   <dimension ref="A1:Q38"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D3" sqref="A3:XFD4"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -36989,7 +36989,7 @@
       <formula1>"genetically manipulated source, natural source, synthetic source"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I5:I1048576" xr:uid="{00000000-0002-0000-0300-000003000000}">
-      <formula1>"cyclic-pseudo-peptide,other,peptide nucleic acid,polydeoxyribonucleotide,polydeoxyribonucleotide/polyribonucleotide,polypeptide(D),polypeptide(L),polyribonucleotide,polysaccharide(D),polysaccharide(L),N/A"</formula1>
+      <formula1>IHM_entity_polymer_type</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix selection choices in Excel sheet
Fix selection choices in Excel sheet for Modeling_protocol (Yes/No)
</commit_message>
<xml_diff>
--- a/example/excel_example.xlsx
+++ b/example/excel_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\excel2mmcif\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5189C1-F95B-4EDA-928A-AE314F4C6A39}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5D9535-6A53-4A5A-BD33-78E7954CE446}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9420" tabRatio="730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4635,7 +4635,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4724,7 +4724,7 @@
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4909,7 +4909,7 @@
         <v>1000</v>
       </c>
       <c r="K5" s="83" t="s">
-        <v>957</v>
+        <v>143</v>
       </c>
       <c r="L5" s="83" t="s">
         <v>958</v>
@@ -4954,7 +4954,7 @@
         <v>1000</v>
       </c>
       <c r="K6" s="83" t="s">
-        <v>957</v>
+        <v>143</v>
       </c>
       <c r="L6" s="83" t="s">
         <v>958</v>
@@ -4973,7 +4973,7 @@
       <c r="O8" s="2"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O1048576" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>Software_id</formula1>
     </dataValidation>
@@ -4982,6 +4982,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D1048576" xr:uid="{00000000-0002-0000-0900-000002000000}">
       <formula1>structure_assembly_id</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K5:K1048576 L5:L1048576 M5:M1048576 N5:N1048576" xr:uid="{D23FAE43-2C63-44D9-BF2D-2903DD20633F}">
+      <formula1>Yes_no_selection</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -36092,8 +36095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:W23"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>